<commit_message>
Checkin of Week 9 documents.
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -35,9 +35,6 @@
     <t>bettich01</t>
   </si>
   <si>
-    <t>March 26 2017</t>
-  </si>
-  <si>
     <t>Illness</t>
   </si>
   <si>
@@ -47,24 +44,15 @@
     <t>dahlda01</t>
   </si>
   <si>
-    <t>May 08 2017</t>
-  </si>
-  <si>
     <t>Ribs</t>
   </si>
   <si>
-    <t>Dahl is on the 10-day disabled list with a stress reaction of his sixth rib and is without a timetable for return.</t>
-  </si>
-  <si>
     <t>Jon Gray</t>
   </si>
   <si>
     <t>grayjo02</t>
   </si>
   <si>
-    <t>May 18 2017</t>
-  </si>
-  <si>
     <t>Toe</t>
   </si>
   <si>
@@ -74,9 +62,6 @@
     <t>murphto04</t>
   </si>
   <si>
-    <t>May 02 2017</t>
-  </si>
-  <si>
     <t>Wrist</t>
   </si>
   <si>
@@ -92,16 +77,55 @@
     <t>PlayerID</t>
   </si>
   <si>
-    <t>Bettis has been designated for the 60-day disabled list as he has been diagnosed with testicular 
-cancer but is expected to return at some point during season as he has started chemotherapy.</t>
-  </si>
-  <si>
-    <t>Gray has been placed on the 10-day disabled list with a stress fracture in his left foot and is 
-expected to be sidelined until the middle of June.</t>
-  </si>
-  <si>
-    <t>Murphy is on the 10-day disabled list while he recovers from a hairline fracture in his wrist. He is 
-expected to be sidelined until sometime in June.</t>
+    <t>Tyler Anderson</t>
+  </si>
+  <si>
+    <t>anderty01</t>
+  </si>
+  <si>
+    <t>June 03 2017</t>
+  </si>
+  <si>
+    <t>Knee</t>
+  </si>
+  <si>
+    <t>Anderson has been placed on the 10-day disabled list with knee inflammation it is unknown when he will rejoin the team.</t>
+  </si>
+  <si>
+    <t>May 29 2017</t>
+  </si>
+  <si>
+    <t>Dahl is on the 10-day disabled list with a stress reaction of his sixth rib and is likely to remain sidelined until sometime in June.</t>
+  </si>
+  <si>
+    <t>June 01 2017</t>
+  </si>
+  <si>
+    <t>Gray has been placed on the 10-day disabled list with a stress fracture in his left foot and is expected to be sidelined until the end of June.</t>
+  </si>
+  <si>
+    <t>May 30 2017</t>
+  </si>
+  <si>
+    <t>Adam Ottavino</t>
+  </si>
+  <si>
+    <t>ottavad01</t>
+  </si>
+  <si>
+    <t>Shoulder</t>
+  </si>
+  <si>
+    <t>Bettis is on the 60-day disabled list while recovering from testicular cancer and it is unknown as to when 
+he will be ready to rejoin the team.</t>
+  </si>
+  <si>
+    <t>Murphy is on the 10-day disabled list while he recovers from a hairline fracture in his wrist but is expected to 
+return by the end of June.</t>
+  </si>
+  <si>
+    <t>Ottavino has been placed on the 10-day disabled list with a inflammation in his right shoulder and is without 
+a timetable for return.</t>
   </si>
 </sst>
 </file>
@@ -137,11 +161,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,18 +481,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -475,64 +501,64 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>23</v>
@@ -540,22 +566,57 @@
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Checkin for Week 11 Newsletter
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23355" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23360" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -56,15 +56,6 @@
     <t>Toe</t>
   </si>
   <si>
-    <t>Tom Murphy</t>
-  </si>
-  <si>
-    <t>murphto04</t>
-  </si>
-  <si>
-    <t>Wrist</t>
-  </si>
-  <si>
     <t>Injury.Type</t>
   </si>
   <si>
@@ -83,49 +74,62 @@
     <t>anderty01</t>
   </si>
   <si>
-    <t>June 03 2017</t>
-  </si>
-  <si>
     <t>Knee</t>
   </si>
   <si>
-    <t>Anderson has been placed on the 10-day disabled list with knee inflammation it is unknown when he will rejoin the team.</t>
-  </si>
-  <si>
-    <t>May 29 2017</t>
-  </si>
-  <si>
     <t>Dahl is on the 10-day disabled list with a stress reaction of his sixth rib and is likely to remain sidelined until sometime in June.</t>
   </si>
   <si>
-    <t>June 01 2017</t>
-  </si>
-  <si>
-    <t>Gray has been placed on the 10-day disabled list with a stress fracture in his left foot and is expected to be sidelined until the end of June.</t>
-  </si>
-  <si>
-    <t>May 30 2017</t>
-  </si>
-  <si>
-    <t>Adam Ottavino</t>
-  </si>
-  <si>
-    <t>ottavad01</t>
-  </si>
-  <si>
-    <t>Shoulder</t>
-  </si>
-  <si>
-    <t>Bettis is on the 60-day disabled list while recovering from testicular cancer and it is unknown as to when 
-he will be ready to rejoin the team.</t>
-  </si>
-  <si>
-    <t>Murphy is on the 10-day disabled list while he recovers from a hairline fracture in his wrist but is expected to 
-return by the end of June.</t>
-  </si>
-  <si>
-    <t>Ottavino has been placed on the 10-day disabled list with a inflammation in his right shoulder and is without 
-a timetable for return.</t>
+    <t>June 12 2017</t>
+  </si>
+  <si>
+    <t>Anderson has been placed on the 10-day disabled list with knee inflammation but is likely to return to the starting rotation before the end of June.</t>
+  </si>
+  <si>
+    <t>June 06 2017</t>
+  </si>
+  <si>
+    <t>Bettis is on the 60-day disabled list while recovering from testicular cancer but is expected to make his season debut sometime around the All-Star break.</t>
+  </si>
+  <si>
+    <t>June 11 2017</t>
+  </si>
+  <si>
+    <t>June 16 2017</t>
+  </si>
+  <si>
+    <t>Gray was placed on the 10-day disabled list with a stress fracture in his left foot. He is on a rehab assignment and is expected to rejoin the rotation during the end of June.</t>
+  </si>
+  <si>
+    <t>Gerardo Parra</t>
+  </si>
+  <si>
+    <t>parrage01</t>
+  </si>
+  <si>
+    <t>June 07 2017</t>
+  </si>
+  <si>
+    <t>Quadricep</t>
+  </si>
+  <si>
+    <t>Parra has landed on the 10-day disabled list with a strained right quadriceps and is likely to be sidelined until the end of June.</t>
+  </si>
+  <si>
+    <t>Chad Qualls</t>
+  </si>
+  <si>
+    <t>quallch01</t>
+  </si>
+  <si>
+    <t>June 18 2017</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Qualls has been placed on the 10-day disabled list with lower back spasms and it is unclear how much time he is 
+expected to miss.</t>
   </si>
 </sst>
 </file>
@@ -484,53 +488,53 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.54296875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -538,16 +542,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -561,10 +565,10 @@
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -572,47 +576,47 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1" t="s">
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkin for the Week 12 newsletter.
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -68,68 +68,64 @@
     <t>PlayerID</t>
   </si>
   <si>
-    <t>Tyler Anderson</t>
-  </si>
-  <si>
-    <t>anderty01</t>
-  </si>
-  <si>
-    <t>Knee</t>
-  </si>
-  <si>
-    <t>Dahl is on the 10-day disabled list with a stress reaction of his sixth rib and is likely to remain sidelined until sometime in June.</t>
-  </si>
-  <si>
-    <t>June 12 2017</t>
-  </si>
-  <si>
-    <t>Anderson has been placed on the 10-day disabled list with knee inflammation but is likely to return to the starting rotation before the end of June.</t>
-  </si>
-  <si>
     <t>June 06 2017</t>
   </si>
   <si>
     <t>Bettis is on the 60-day disabled list while recovering from testicular cancer but is expected to make his season debut sometime around the All-Star break.</t>
   </si>
   <si>
-    <t>June 11 2017</t>
-  </si>
-  <si>
-    <t>June 16 2017</t>
-  </si>
-  <si>
-    <t>Gray was placed on the 10-day disabled list with a stress fracture in his left foot. He is on a rehab assignment and is expected to rejoin the rotation during the end of June.</t>
-  </si>
-  <si>
     <t>Gerardo Parra</t>
   </si>
   <si>
     <t>parrage01</t>
   </si>
   <si>
-    <t>June 07 2017</t>
-  </si>
-  <si>
     <t>Quadricep</t>
   </si>
   <si>
-    <t>Parra has landed on the 10-day disabled list with a strained right quadriceps and is likely to be sidelined until the end of June.</t>
-  </si>
-  <si>
     <t>Chad Qualls</t>
   </si>
   <si>
     <t>quallch01</t>
   </si>
   <si>
-    <t>June 18 2017</t>
-  </si>
-  <si>
     <t>Back</t>
   </si>
   <si>
-    <t>Qualls has been placed on the 10-day disabled list with lower back spasms and it is unclear how much time he is 
-expected to miss.</t>
+    <t>June 23 2017</t>
+  </si>
+  <si>
+    <t>Dahl is on the 10-day disabled list with a stress reaction of his sixth rib. It is unknown as to when he will be ready to join the lineup.</t>
+  </si>
+  <si>
+    <t>Carlos Gonzalez</t>
+  </si>
+  <si>
+    <t>gonzaca01</t>
+  </si>
+  <si>
+    <t>June 25 2017</t>
+  </si>
+  <si>
+    <t>Shoulder</t>
+  </si>
+  <si>
+    <t>Gonzalez has missed the last two games with a sore right shoulder and his status is uncertain for Sunday's game against the Dodgers.</t>
+  </si>
+  <si>
+    <t>June 20 2017</t>
+  </si>
+  <si>
+    <t>Gray was placed on the 10-day disabled list with a stress fracture in his left foot. He is on a rehab assignment and is expected to rejoin the rotation before the beginning of July.</t>
+  </si>
+  <si>
+    <t>Parra has landed on the 10-day disabled list with a strained right quadriceps and is likely to be sidelined until the start of July.</t>
+  </si>
+  <si>
+    <t>June 21 2017</t>
+  </si>
+  <si>
+    <t>Qualls has been placed on the 10-day disabled list with lower back spasms and it is unclear as to if he will return for Monday's game against the Giants.</t>
   </si>
 </sst>
 </file>
@@ -488,7 +484,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -519,53 +515,53 @@
     </row>
     <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -576,47 +572,47 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
       </c>
       <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkin Week 14 newsletter.
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -65,24 +65,6 @@
     <t>Bettis is on the 60-day disabled list while recovering from testicular cancer but is expected to make his season debut sometime around the All-Star break.</t>
   </si>
   <si>
-    <t>Gerardo Parra</t>
-  </si>
-  <si>
-    <t>parrage01</t>
-  </si>
-  <si>
-    <t>Quadricep</t>
-  </si>
-  <si>
-    <t>Carlos Gonzalez</t>
-  </si>
-  <si>
-    <t>gonzaca01</t>
-  </si>
-  <si>
-    <t>Shoulder</t>
-  </si>
-  <si>
     <t>Tyler Anderson</t>
   </si>
   <si>
@@ -101,15 +83,6 @@
     <t>Dahl has been moved to the 60-day disabled list with a stress reaction of his sixth rib and it is unknown as to when he will be ready to join the lineup.</t>
   </si>
   <si>
-    <t>June 26 2017</t>
-  </si>
-  <si>
-    <t>Gonzalez has been placed on the 10-day disabled list with a sore right shoulder and is without a clear timetable for a recovery.</t>
-  </si>
-  <si>
-    <t>July 02 2017</t>
-  </si>
-  <si>
     <t>Ian Desmond</t>
   </si>
   <si>
@@ -119,10 +92,10 @@
     <t>Calf</t>
   </si>
   <si>
-    <t>Desmond departed the previous game due to cramping in his right calf and his status is uncertain for Monday's game against the Reds.</t>
-  </si>
-  <si>
-    <t>Parra has landed on the 10-day disabled list with a strained right quadriceps and will likely remain sidelined until the All-Star break.</t>
+    <t>July 03 2017</t>
+  </si>
+  <si>
+    <t>Desmond has landed on the 10-day disabled list with a right calf strain and it is unknown as to how long he will be out of action.</t>
   </si>
 </sst>
 </file>
@@ -478,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -512,19 +485,19 @@
     </row>
     <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -552,64 +525,30 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkin for Week #15.
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23360" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23355" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,12 +59,6 @@
     <t>PlayerID</t>
   </si>
   <si>
-    <t>June 06 2017</t>
-  </si>
-  <si>
-    <t>Bettis is on the 60-day disabled list while recovering from testicular cancer but is expected to make his season debut sometime around the All-Star break.</t>
-  </si>
-  <si>
     <t>Tyler Anderson</t>
   </si>
   <si>
@@ -83,19 +77,25 @@
     <t>Dahl has been moved to the 60-day disabled list with a stress reaction of his sixth rib and it is unknown as to when he will be ready to join the lineup.</t>
   </si>
   <si>
-    <t>Ian Desmond</t>
-  </si>
-  <si>
-    <t>desmoia01</t>
-  </si>
-  <si>
     <t>Calf</t>
   </si>
   <si>
-    <t>July 03 2017</t>
-  </si>
-  <si>
-    <t>Desmond has landed on the 10-day disabled list with a right calf strain and it is unknown as to how long he will be out of action.</t>
+    <t>July 10 2017</t>
+  </si>
+  <si>
+    <t>Bettis is on the 60-day disabled list while recovering from testicular cancer but is expected to make his season debut sometime during the later part of July.</t>
+  </si>
+  <si>
+    <t>Tyler Chatwood</t>
+  </si>
+  <si>
+    <t>chatwty01</t>
+  </si>
+  <si>
+    <t>July 16 2017</t>
+  </si>
+  <si>
+    <t>Chatwood has been placed on the 10-day disabled list with a right calf strain and there is no timetable for return.</t>
   </si>
 </sst>
 </file>
@@ -454,19 +454,19 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,24 +483,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -508,47 +508,47 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkin for Week #16 Newsletter
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -38,15 +38,6 @@
     <t>Illness</t>
   </si>
   <si>
-    <t>David Dahl</t>
-  </si>
-  <si>
-    <t>dahlda01</t>
-  </si>
-  <si>
-    <t>Ribs</t>
-  </si>
-  <si>
     <t>Injury.Type</t>
   </si>
   <si>
@@ -65,27 +56,12 @@
     <t>anderty01</t>
   </si>
   <si>
-    <t>June 27 2017</t>
-  </si>
-  <si>
     <t>Knee</t>
   </si>
   <si>
-    <t>Anderson has been designated for the 10-day disabled list as he will have arthroscopic left knee surgery and is expected to miss up to four weeks of action.</t>
-  </si>
-  <si>
-    <t>Dahl has been moved to the 60-day disabled list with a stress reaction of his sixth rib and it is unknown as to when he will be ready to join the lineup.</t>
-  </si>
-  <si>
     <t>Calf</t>
   </si>
   <si>
-    <t>July 10 2017</t>
-  </si>
-  <si>
-    <t>Bettis is on the 60-day disabled list while recovering from testicular cancer but is expected to make his season debut sometime during the later part of July.</t>
-  </si>
-  <si>
     <t>Tyler Chatwood</t>
   </si>
   <si>
@@ -96,18 +72,47 @@
   </si>
   <si>
     <t>Chatwood has been placed on the 10-day disabled list with a right calf strain and there is no timetable for return.</t>
+  </si>
+  <si>
+    <t>July 21 2017</t>
+  </si>
+  <si>
+    <t>Anderson has been designated for the 10-day disabled list as he will have arthroscopic left knee surgery and is expected to be sidelined until the beginning of August.</t>
+  </si>
+  <si>
+    <t>Bettis is on the 60-day disabled list while recovering from testicular cancer but is expected to make his season debut sometime during the early part of August.</t>
+  </si>
+  <si>
+    <t>Gerardo Parra</t>
+  </si>
+  <si>
+    <t>parrage01</t>
+  </si>
+  <si>
+    <t>July 23 2017</t>
+  </si>
+  <si>
+    <t>Parra sat out the previous game due to a right calf contusion and it is unclear as to if he will play against the Cardinals on Monday.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -131,12 +136,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +462,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,84 +479,84 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
+      <c r="A2" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
+      <c r="A4" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
+      <c r="A5" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkin for Week #17.
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -62,37 +62,43 @@
     <t>Calf</t>
   </si>
   <si>
-    <t>Tyler Chatwood</t>
-  </si>
-  <si>
-    <t>chatwty01</t>
-  </si>
-  <si>
-    <t>July 16 2017</t>
-  </si>
-  <si>
-    <t>Chatwood has been placed on the 10-day disabled list with a right calf strain and there is no timetable for return.</t>
-  </si>
-  <si>
     <t>July 21 2017</t>
   </si>
   <si>
-    <t>Anderson has been designated for the 10-day disabled list as he will have arthroscopic left knee surgery and is expected to be sidelined until the beginning of August.</t>
-  </si>
-  <si>
     <t>Bettis is on the 60-day disabled list while recovering from testicular cancer but is expected to make his season debut sometime during the early part of August.</t>
   </si>
   <si>
-    <t>Gerardo Parra</t>
-  </si>
-  <si>
-    <t>parrage01</t>
-  </si>
-  <si>
-    <t>July 23 2017</t>
-  </si>
-  <si>
-    <t>Parra sat out the previous game due to a right calf contusion and it is unclear as to if he will play against the Cardinals on Monday.</t>
+    <t>July 27 2017</t>
+  </si>
+  <si>
+    <t>Anderson has been transferred to the 60-day disabled list due to arthroscopic left knee surgery and is expected to be sidelined until the end of August.</t>
+  </si>
+  <si>
+    <t>Ian Desmond</t>
+  </si>
+  <si>
+    <t>desmoia01</t>
+  </si>
+  <si>
+    <t>July 28 2017</t>
+  </si>
+  <si>
+    <t>Desmond has been placed on the 10-day disabled due to a right calf strain. A timetable for his recovery has yet to be established.</t>
+  </si>
+  <si>
+    <t>Jake McGee</t>
+  </si>
+  <si>
+    <t>mcgeeja01</t>
+  </si>
+  <si>
+    <t>July 30 2017</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>McGee has been placed on the 10-day disabled list with a back injury and it is unclear how much time he is expected to miss.</t>
   </si>
 </sst>
 </file>
@@ -462,7 +468,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,13 +505,13 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -516,47 +522,47 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkin of Week19 newsletter.
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -71,54 +71,31 @@
     <t>Desmond has been placed on the 10-day disabled due to a right calf strain. A timetable for his recovery has yet to be established.</t>
   </si>
   <si>
-    <t>Jake McGee</t>
-  </si>
-  <si>
-    <t>mcgeeja01</t>
-  </si>
-  <si>
-    <t>Back</t>
-  </si>
-  <si>
     <t>Kyle Freeland</t>
   </si>
   <si>
     <t>freelky01</t>
   </si>
   <si>
-    <t>August 05 2017</t>
-  </si>
-  <si>
     <t>Groin</t>
   </si>
   <si>
-    <t>Freeland is on the 10-day disabled list with a left groin strain and is expected to need three-to-four weeks to recover.</t>
-  </si>
-  <si>
-    <t>August 03 2017</t>
-  </si>
-  <si>
-    <t>McGee is on the 10-day disabled list with a mid-back strain. It is unknown if he will be activated for the upcoming series against the Indians that begins Tuesday.</t>
+    <t>August 09 2017</t>
+  </si>
+  <si>
+    <t>Freeland is on the 10-day disabled list with a left groin strain and is expected to remain sidelined until the end of August.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -142,15 +119,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,17 +439,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="98.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
@@ -498,7 +472,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
@@ -515,7 +489,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
@@ -532,37 +506,20 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkin changes made for Week #20.
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -69,21 +69,6 @@
   </si>
   <si>
     <t>Desmond has been placed on the 10-day disabled due to a right calf strain. A timetable for his recovery has yet to be established.</t>
-  </si>
-  <si>
-    <t>Kyle Freeland</t>
-  </si>
-  <si>
-    <t>freelky01</t>
-  </si>
-  <si>
-    <t>Groin</t>
-  </si>
-  <si>
-    <t>August 09 2017</t>
-  </si>
-  <si>
-    <t>Freeland is on the 10-day disabled list with a left groin strain and is expected to remain sidelined until the end of August.</t>
   </si>
 </sst>
 </file>
@@ -439,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A4" sqref="A4:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,23 +490,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed Week 21 newsletter.
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23355" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23360" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -53,12 +53,6 @@
     <t>Calf</t>
   </si>
   <si>
-    <t>July 27 2017</t>
-  </si>
-  <si>
-    <t>Anderson has been transferred to the 60-day disabled list due to arthroscopic left knee surgery and is expected to be sidelined until the end of August.</t>
-  </si>
-  <si>
     <t>Ian Desmond</t>
   </si>
   <si>
@@ -69,12 +63,33 @@
   </si>
   <si>
     <t>Desmond has been placed on the 10-day disabled due to a right calf strain. A timetable for his recovery has yet to be established.</t>
+  </si>
+  <si>
+    <t>August 21 2017</t>
+  </si>
+  <si>
+    <t>Anderson has been transferred to the 60-day disabled list due to arthroscopic left knee surgery and is expected to be sidelined until the start of September.</t>
+  </si>
+  <si>
+    <t>August 22 2017</t>
+  </si>
+  <si>
+    <t>Groin</t>
+  </si>
+  <si>
+    <t>Hanigan is on the 10-day disabled list with a left groin strain and will miss an undetermined amount of game action.</t>
+  </si>
+  <si>
+    <t>Ryan Hanigan</t>
+  </si>
+  <si>
+    <t>hanigry01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -423,23 +438,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD8"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.54296875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -464,30 +479,47 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Week #23 Newsletter.
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -41,34 +41,19 @@
     <t>PlayerID</t>
   </si>
   <si>
-    <t>Tyler Anderson</t>
-  </si>
-  <si>
-    <t>anderty01</t>
-  </si>
-  <si>
-    <t>Knee</t>
-  </si>
-  <si>
-    <t>August 22 2017</t>
-  </si>
-  <si>
-    <t>Groin</t>
-  </si>
-  <si>
-    <t>Hanigan is on the 10-day disabled list with a left groin strain and will miss an undetermined amount of game action.</t>
-  </si>
-  <si>
-    <t>Ryan Hanigan</t>
-  </si>
-  <si>
-    <t>hanigry01</t>
-  </si>
-  <si>
-    <t>September 02 2017</t>
-  </si>
-  <si>
-    <t>Anderson has been transferred to the 60-day disabled list due to arthroscopic left knee surgery and is expected to be sidelined until the middle of September.</t>
+    <t>Jairo Diaz</t>
+  </si>
+  <si>
+    <t>diazja01</t>
+  </si>
+  <si>
+    <t>September 10 2017</t>
+  </si>
+  <si>
+    <t>Undisclosed</t>
+  </si>
+  <si>
+    <t>Diaz is on the 60-day disabled list with an unknown injury ending his season.</t>
   </si>
 </sst>
 </file>
@@ -424,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -464,30 +449,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Week 25 newsletter.
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -47,13 +47,40 @@
     <t>diazja01</t>
   </si>
   <si>
-    <t>September 10 2017</t>
-  </si>
-  <si>
-    <t>Undisclosed</t>
-  </si>
-  <si>
-    <t>Diaz is on the 60-day disabled list with an unknown injury ending his season.</t>
+    <t>September 12 2017</t>
+  </si>
+  <si>
+    <t>Elbow</t>
+  </si>
+  <si>
+    <t>Diaz is on the 60-day disabled list with inflammation in his left elbow and will miss the remainder of the season.</t>
+  </si>
+  <si>
+    <t>Nolan Arenado</t>
+  </si>
+  <si>
+    <t>arenano01</t>
+  </si>
+  <si>
+    <t>September 24 2017</t>
+  </si>
+  <si>
+    <t>Hand</t>
+  </si>
+  <si>
+    <t>Arenado is dealing with a bruised right hand near his thumb and his status for Monday's contest against the Marlins is undetermined.</t>
+  </si>
+  <si>
+    <t>Carlos Gonzalez</t>
+  </si>
+  <si>
+    <t>gonzaca01</t>
+  </si>
+  <si>
+    <t>Shoulder</t>
+  </si>
+  <si>
+    <t>Gonzalez sat out the last game due to a shoulder injury and his availability for Monday's tilt against the Marlins is undecided.</t>
   </si>
 </sst>
 </file>
@@ -409,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,22 +468,62 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Checkin Rockies 2018 Wk07.
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdreed\Desktop\MyProjects\Rockies\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdreed\Desktop\MyProjects\Rockies18\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AA0F54-9A65-4EBB-82DB-064427DBEE31}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23355" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -41,46 +42,49 @@
     <t>PlayerID</t>
   </si>
   <si>
-    <t>Jairo Diaz</t>
-  </si>
-  <si>
-    <t>diazja01</t>
-  </si>
-  <si>
-    <t>September 12 2017</t>
-  </si>
-  <si>
-    <t>Elbow</t>
-  </si>
-  <si>
-    <t>Diaz is on the 60-day disabled list with inflammation in his left elbow and will miss the remainder of the season.</t>
-  </si>
-  <si>
-    <t>Nolan Arenado</t>
-  </si>
-  <si>
-    <t>arenano01</t>
-  </si>
-  <si>
-    <t>September 24 2017</t>
-  </si>
-  <si>
-    <t>Hand</t>
-  </si>
-  <si>
-    <t>Arenado is dealing with a bruised right hand near his thumb and his status for Monday's contest against the Marlins is undetermined.</t>
-  </si>
-  <si>
-    <t>Carlos Gonzalez</t>
-  </si>
-  <si>
-    <t>gonzaca01</t>
-  </si>
-  <si>
-    <t>Shoulder</t>
-  </si>
-  <si>
-    <t>Gonzalez sat out the last game due to a shoulder injury and his availability for Monday's tilt against the Marlins is undecided.</t>
+    <t>Oblique</t>
+  </si>
+  <si>
+    <t>Finger</t>
+  </si>
+  <si>
+    <t>Carlos Estevez</t>
+  </si>
+  <si>
+    <t>estevca01</t>
+  </si>
+  <si>
+    <t>Zac Rosscup</t>
+  </si>
+  <si>
+    <t>rosscza01</t>
+  </si>
+  <si>
+    <t>April 23 2018</t>
+  </si>
+  <si>
+    <t>Estevez has been shifted to the 60-day disabled list due to a left oblique strain but is likely to return during the latter part of May.</t>
+  </si>
+  <si>
+    <t>May 01 2018</t>
+  </si>
+  <si>
+    <t>Rosscup has been shifted to the 60-day disabled list dealing with warts on his left middle finger and is likely to stay on the DL until at least the end of May.</t>
+  </si>
+  <si>
+    <t>DJ LeMahieu</t>
+  </si>
+  <si>
+    <t>lemahdj01</t>
+  </si>
+  <si>
+    <t>May 18 2018</t>
+  </si>
+  <si>
+    <t>Wrist</t>
+  </si>
+  <si>
+    <t>LeMahieu is on the 10-day disabled list after being diagnosed with a slight left wrist fracture and a sprained thumb. There is no timetable for return.</t>
   </si>
 </sst>
 </file>
@@ -436,19 +440,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="98.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -468,62 +472,56 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="1"/>
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Week #13 partial + Week #14 start.
</commit_message>
<xml_diff>
--- a/data/Rockies_Injuries.xlsx
+++ b/data/Rockies_Injuries.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdreed\Desktop\MyProjects\Rockies18\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdree\Desktop\MyProjects\Rockies18\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AA0F54-9A65-4EBB-82DB-064427DBEE31}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA1C14B-02BA-464A-8EEA-5F17689641B0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23355" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -60,31 +60,52 @@
     <t>rosscza01</t>
   </si>
   <si>
-    <t>April 23 2018</t>
-  </si>
-  <si>
-    <t>Estevez has been shifted to the 60-day disabled list due to a left oblique strain but is likely to return during the latter part of May.</t>
-  </si>
-  <si>
-    <t>May 01 2018</t>
-  </si>
-  <si>
-    <t>Rosscup has been shifted to the 60-day disabled list dealing with warts on his left middle finger and is likely to stay on the DL until at least the end of May.</t>
-  </si>
-  <si>
-    <t>DJ LeMahieu</t>
-  </si>
-  <si>
-    <t>lemahdj01</t>
-  </si>
-  <si>
-    <t>May 18 2018</t>
-  </si>
-  <si>
-    <t>Wrist</t>
-  </si>
-  <si>
-    <t>LeMahieu is on the 10-day disabled list after being diagnosed with a slight left wrist fracture and a sprained thumb. There is no timetable for return.</t>
+    <t>Chad Bettis</t>
+  </si>
+  <si>
+    <t>bettich01</t>
+  </si>
+  <si>
+    <t>July 01 2018</t>
+  </si>
+  <si>
+    <t>Bettis left his last outing due to a right middle finger injury and it is unknown if he will make his next scheduled start Saturday against the Mariners.</t>
+  </si>
+  <si>
+    <t>David Dahl</t>
+  </si>
+  <si>
+    <t>dahlda01</t>
+  </si>
+  <si>
+    <t>June 02 2018</t>
+  </si>
+  <si>
+    <t>Foot</t>
+  </si>
+  <si>
+    <t>Dahl has been placed on the 10-day disabled list with a broken right foot and will likely need six-to-eight weeks to recover.</t>
+  </si>
+  <si>
+    <t>Estevez has been shifted to the 60-day disabled list due to a left oblique strain but is likely to return during the middle portion of July.</t>
+  </si>
+  <si>
+    <t>Rosscup has been shifted to the 60-day disabled list dealing with warts on his left middle finger and is likely to stay on the DL until at least the middle of July.</t>
+  </si>
+  <si>
+    <t>Bryan Shaw</t>
+  </si>
+  <si>
+    <t>shawbr01</t>
+  </si>
+  <si>
+    <t>June 24 2018</t>
+  </si>
+  <si>
+    <t>Calf</t>
+  </si>
+  <si>
+    <t>Shaw has landed on the 10-day disables list with a right calf strain and there is no timetable for return.</t>
   </si>
 </sst>
 </file>
@@ -440,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,19 +495,19 @@
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -508,19 +529,53 @@
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>